<commit_message>
changes done by master
</commit_message>
<xml_diff>
--- a/src/test/resources/FetchFromExcel.xlsx
+++ b/src/test/resources/FetchFromExcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAPPU YADAV\Desktop\work\Zolanda_Online_Shopping_Selenium_Framework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3287BFFF-2D0E-40DF-8C8C-219C9849D5D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C360CA5-003A-439B-981D-4F547FD3137A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="9" xr2:uid="{C2F0BF46-E3F7-481B-8BEA-EC7569DC8E9A}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="119">
   <si>
     <t>url</t>
   </si>
@@ -393,6 +393,12 @@
   </si>
   <si>
     <t>rama@123gmail.com</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>ap</t>
   </si>
 </sst>
 </file>
@@ -491,7 +497,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -510,6 +516,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -938,10 +945,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{734EDF4A-1AA5-4825-B67D-3C6D30A09EAE}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,6 +980,22 @@
       </c>
       <c r="B3" s="1" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>